<commit_message>
Train-006 Update for SH team tranining.
</commit_message>
<xml_diff>
--- a/training Schedule_forCDP.xlsx
+++ b/training Schedule_forCDP.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="SHTeam2016" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Work Order</t>
   </si>
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,12 +716,162 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4">
+        <v>41661</v>
+      </c>
+      <c r="C2" s="5">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4">
+        <v>41662</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="255" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="5">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4">
+        <v>41666</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4">
+        <v>41667</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Train-007 added some file, including TaiWan project.
</commit_message>
<xml_diff>
--- a/training Schedule_forCDP.xlsx
+++ b/training Schedule_forCDP.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -718,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>